<commit_message>
added test plan + bug report
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -10,59 +10,286 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="K2">
+      <text>
+        <t xml:space="preserve">we will need to fill this part in as well
+	-Andie Lizo</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Bug</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="84">
+  <si>
+    <t>Bug #</t>
+  </si>
+  <si>
+    <t>Reported Date</t>
+  </si>
+  <si>
+    <t>Reported By</t>
   </si>
   <si>
     <t>Priority</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>Owner</t>
   </si>
   <si>
-    <t>Status</t>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual Results </t>
   </si>
   <si>
     <t>Milestone</t>
   </si>
   <si>
-    <t>Deliverable</t>
-  </si>
-  <si>
-    <t>Notes</t>
+    <t>Steps to Reproduce</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Andie</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Avi Sharma</t>
+  </si>
+  <si>
+    <t>Sounds for picking up keys or dying  is not being played if the wall collision is play at the same time</t>
+  </si>
+  <si>
+    <t>The key pick up sound or dying sound should play</t>
+  </si>
+  <si>
+    <t>You should be able to play multiple sound effects on top of another</t>
+  </si>
+  <si>
+    <t>Milestone 1</t>
+  </si>
+  <si>
+    <t>If the key is near an obstacle (trees/stones), press the WASD key accordingly to move into the wall and press the E key to pick up the key or wait for robot to collide with the player.</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>P0</t>
   </si>
   <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Collision with trees on top results in an error</t>
+  </si>
+  <si>
+    <t>Collision with tress on top should play a sound</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Andie/Avi</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>Song Shi</t>
+  </si>
+  <si>
+    <t>BFS does not work if the player is in line with the robot (when an object is in line and in between the robot and player)</t>
+  </si>
+  <si>
+    <t>The robot moves towards the player</t>
+  </si>
+  <si>
+    <t>The robot gets stuck at the obstacles</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Zeen</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
     <t>Not started</t>
   </si>
   <si>
+    <t>Zeen Lin</t>
+  </si>
+  <si>
+    <t>Visual effects could be improved to be more realistic when the player moves to the tree tiles</t>
+  </si>
+  <si>
+    <t>The tree leaves visually cover some parts of the player's body</t>
+  </si>
+  <si>
+    <t>The tree leaves are not visually covering the player body when the player stands on the tree tiles</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>P1</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>Blocked</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>Completed</t>
+    <t>Keys spawning in walls not accessible by players</t>
+  </si>
+  <si>
+    <t>Keys spawning outside walls and accessible by players</t>
+  </si>
+  <si>
+    <t>Random spawning of keys made the keys not accessible by players.</t>
+  </si>
+  <si>
+    <t>Milestone 2</t>
+  </si>
+  <si>
+    <t>set spawn locations</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Robots spawning in walls and not able to move out</t>
+  </si>
+  <si>
+    <t>Robots to spawn outside the walls and move around</t>
+  </si>
+  <si>
+    <t>Random spawning makes robot spawn inside the walls and not be able to move</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Player walking animation stops even if the player is still walking</t>
+  </si>
+  <si>
+    <t>Player should keep walking animation when walking</t>
+  </si>
+  <si>
+    <t>Player only does first 2 frames of walking animation when WASD is initially pressed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fix logic for animation </t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Avi</t>
+  </si>
+  <si>
+    <t>Andie Lizo</t>
+  </si>
+  <si>
+    <t>Player health bar - current health gets set to 0 when - key is pressed</t>
+  </si>
+  <si>
+    <t>Current health value should decrease by 10</t>
+  </si>
+  <si>
+    <t>Current health value gets set to 0</t>
+  </si>
+  <si>
+    <t>change from int to float</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>When player is walking - then attacking is not possible</t>
+  </si>
+  <si>
+    <t>Player should be able to attack (go through attack animation)</t>
+  </si>
+  <si>
+    <t>Player keeps walking</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Player Inventory is erased when moving to another level</t>
+  </si>
+  <si>
+    <t>Inventory contents should remain the same thoughout levels (unless the player dies)</t>
+  </si>
+  <si>
+    <t>Inventory contents go away after moving to next level</t>
+  </si>
+  <si>
+    <t>keep inventory in registry when loading new level</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Song</t>
+  </si>
+  <si>
+    <t>Player attacking up instantly kills the robot</t>
+  </si>
+  <si>
+    <t>Player attacking the robot in the updward direction should damage the robot but not kill it</t>
+  </si>
+  <si>
+    <t>Robot dies in one shot</t>
+  </si>
+  <si>
+    <t>Move under the robot and then press W key to look up and left click to attack</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projectile hiting the walls sometimes creates a new wall (very infrequently) </t>
+  </si>
+  <si>
+    <t>Projectile should just hit the wall</t>
+  </si>
+  <si>
+    <t>Projectile htting the wall sometimes adds a new wall</t>
+  </si>
+  <si>
+    <t>Not consistent - Moving towards the end and killing the robots and moving back and dodging projectiles created the new wall after impact with the wall.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -74,16 +301,54 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FFFFFFFF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF49564C"/>
+        <bgColor rgb="FF49564C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F8F9"/>
+        <bgColor rgb="FFF6F8F9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border/>
     <border>
       <left style="thin">
@@ -216,10 +481,24 @@
         <color rgb="FF374139"/>
       </left>
       <right style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF374139"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF374139"/>
@@ -241,13 +520,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
         <color rgb="FF374139"/>
       </right>
       <top style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF374139"/>
@@ -257,60 +536,102 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -370,15 +691,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G15" displayName="Project_tasks1" name="Project_tasks1" id="1">
-  <tableColumns count="7">
-    <tableColumn name="Bug" id="1"/>
-    <tableColumn name="Priority" id="2"/>
-    <tableColumn name="Owner" id="3"/>
-    <tableColumn name="Status" id="4"/>
-    <tableColumn name="Milestone" id="5"/>
-    <tableColumn name="Deliverable" id="6"/>
-    <tableColumn name="Notes" id="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:K14" displayName="Project_tasks1" name="Project_tasks1" id="1">
+  <tableColumns count="11">
+    <tableColumn name="Bug #" id="1"/>
+    <tableColumn name="Reported Date" id="2"/>
+    <tableColumn name="Reported By" id="3"/>
+    <tableColumn name="Priority" id="4"/>
+    <tableColumn name="Status" id="5"/>
+    <tableColumn name="Owner" id="6"/>
+    <tableColumn name="Description" id="7"/>
+    <tableColumn name="Expected Results" id="8"/>
+    <tableColumn name="Actual Results " id="9"/>
+    <tableColumn name="Milestone" id="10"/>
+    <tableColumn name="Steps to Reproduce" id="11"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -591,11 +916,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.13"/>
-    <col customWidth="1" min="2" max="4" width="15.13"/>
-    <col customWidth="1" min="5" max="5" width="20.13"/>
-    <col customWidth="1" min="6" max="6" width="22.63"/>
-    <col customWidth="1" min="7" max="7" width="15.13"/>
+    <col customWidth="1" min="1" max="1" width="15.0"/>
+    <col customWidth="1" min="2" max="6" width="15.13"/>
+    <col customWidth="1" min="7" max="7" width="24.63"/>
+    <col customWidth="1" min="8" max="11" width="20.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -605,7 +929,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -617,165 +941,696 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
     </row>
     <row r="2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
+      <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7">
+        <v>45576.0</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
     </row>
     <row r="3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
+      <c r="A3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="16">
+        <v>45577.0</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="22"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
     </row>
     <row r="4">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
+      <c r="A4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="7">
+        <v>45577.0</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
+      <c r="A5" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="16">
+        <v>45577.0</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="22"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
     </row>
     <row r="6">
-      <c r="A6" s="4"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
+      <c r="A6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="7">
+        <v>45594.0</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
     </row>
     <row r="7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
+      <c r="A7" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="16">
+        <v>45594.0</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
     </row>
     <row r="8">
-      <c r="A8" s="4"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
+      <c r="A8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="7">
+        <v>45594.0</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
     </row>
     <row r="9">
-      <c r="A9" s="8"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
+      <c r="A9" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="16">
+        <v>45595.0</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
     </row>
     <row r="10">
-      <c r="A10" s="4"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
+      <c r="A10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="7">
+        <v>45595.0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="14"/>
     </row>
     <row r="11">
-      <c r="A11" s="8"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
+      <c r="A11" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="16">
+        <v>45596.0</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14"/>
     </row>
     <row r="12">
-      <c r="A12" s="4"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
+      <c r="A12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="23">
+        <v>45599.0</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14"/>
     </row>
     <row r="13">
-      <c r="A13" s="8"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="11"/>
+      <c r="A13" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="24">
+        <v>45599.0</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14"/>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="14"/>
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="14"/>
     </row>
     <row r="14">
-      <c r="A14" s="4"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="17"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14"/>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:A15 E2:E15 G2:G15"/>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B15">
-      <formula1>"P0,P1,P2,P3"</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="D2:D14">
+      <formula1>"P5,P4,P3,P2,P1,P0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D15">
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:A14 J2:K14"/>
+    <dataValidation type="list" allowBlank="1" sqref="E2:E14">
       <formula1>"Not started,In progress,Blocked,Completed"</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId2" ref="F2"/>
+    <hyperlink r:id="rId3" ref="F3"/>
+    <hyperlink r:id="rId4" ref="F7"/>
+    <hyperlink r:id="rId5" ref="F8"/>
+    <hyperlink r:id="rId6" ref="F9"/>
+    <hyperlink r:id="rId7" ref="F10"/>
+    <hyperlink r:id="rId8" ref="F11"/>
+  </hyperlinks>
+  <drawing r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>